<commit_message>
Uppfærði to do listann + Effort Estimation Sheet
Bjó til "nýjann" to do lista, þ.e uppfærði hann þannig að það er
einfaldara að sjá hvað vantar að útfæra. Það mesta sem er eftir er
eiginlega bara að setja upp tengingu og prufukeyra þetta allt saman, +
smá auka hlutir.

Uppfærði Effort Estimation Sheet - það er ein user story sem á ekki við
lengur og tveir eða þrír reitir sem ég fyllti ekki út strax, en það
hlýtur að koma inn fljótlega þegar við klárum þetta nú loksins.
</commit_message>
<xml_diff>
--- a/Effort Estimation Sheet.xlsx
+++ b/Effort Estimation Sheet.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>User Story ID</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Additional information</t>
+  </si>
+  <si>
+    <t>Taka út öruglega</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +703,9 @@
       <c r="H4" s="3">
         <v>5</v>
       </c>
+      <c r="I4" s="3">
+        <v>6</v>
+      </c>
       <c r="J4" s="3">
         <v>1</v>
       </c>
@@ -789,6 +795,9 @@
       <c r="H7" s="3">
         <v>13</v>
       </c>
+      <c r="I7" s="3">
+        <v>10</v>
+      </c>
       <c r="J7" s="3">
         <v>2</v>
       </c>
@@ -854,7 +863,9 @@
       <c r="J9" s="3">
         <v>4</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
@@ -957,6 +968,9 @@
       <c r="H13" s="3">
         <v>15</v>
       </c>
+      <c r="I13" s="3">
+        <v>12</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -981,6 +995,9 @@
       <c r="H14" s="3">
         <v>15</v>
       </c>
+      <c r="I14" s="3">
+        <v>10</v>
+      </c>
       <c r="J14" s="3">
         <v>1</v>
       </c>
@@ -1076,6 +1093,9 @@
       <c r="H17" s="3">
         <v>8</v>
       </c>
+      <c r="I17" s="3">
+        <v>5</v>
+      </c>
       <c r="J17" s="3">
         <v>2</v>
       </c>
@@ -1136,6 +1156,9 @@
         <v>1</v>
       </c>
       <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3">
         <v>2</v>
       </c>
       <c r="J19" t="s">

</xml_diff>